<commit_message>
#3149 - แก้ไข error ของ purchase_tracking report
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_tracking.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_tracking.xlsx
@@ -309,10 +309,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,57 +648,58 @@
   <dimension ref="A1:BB33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.75" style="2" customWidth="1"/>
     <col min="4" max="4" width="25.625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17" style="2" customWidth="1"/>
-    <col min="6" max="6" width="25.625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18" style="2" customWidth="1"/>
-    <col min="8" max="8" width="21.875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="23.625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="27.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.75" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17.75" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.75" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13" style="2" customWidth="1"/>
     <col min="13" max="13" width="15.75" style="2" customWidth="1"/>
-    <col min="14" max="14" width="19.375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="16.375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="20.375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="21.25" style="2" customWidth="1"/>
-    <col min="18" max="18" width="25.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="25.875" style="2" customWidth="1"/>
-    <col min="21" max="21" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="13.375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="15.875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="13.875" style="2" customWidth="1"/>
+    <col min="16" max="17" width="15.75" style="2" customWidth="1"/>
+    <col min="18" max="18" width="19.625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="25.25" style="2" customWidth="1"/>
+    <col min="20" max="20" width="24.125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="23.625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="9.25" style="2" customWidth="1"/>
+    <col min="23" max="23" width="33.25" style="2" customWidth="1"/>
+    <col min="24" max="24" width="35" style="2" customWidth="1"/>
     <col min="25" max="25" width="24.75" style="2" customWidth="1"/>
-    <col min="26" max="26" width="24" style="2" customWidth="1"/>
-    <col min="27" max="27" width="17.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.875" style="2" customWidth="1"/>
+    <col min="27" max="27" width="36.25" style="2" customWidth="1"/>
     <col min="28" max="28" width="17.875" style="2" customWidth="1"/>
-    <col min="29" max="29" width="21.375" style="2" customWidth="1"/>
-    <col min="30" max="30" width="22.875" style="2" customWidth="1"/>
-    <col min="31" max="31" width="11.75" style="1" customWidth="1"/>
-    <col min="32" max="32" width="24.75" style="2" customWidth="1"/>
-    <col min="33" max="33" width="15.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.375" style="2" customWidth="1"/>
-    <col min="35" max="35" width="13.25" style="2" customWidth="1"/>
+    <col min="29" max="29" width="12.125" style="2" customWidth="1"/>
+    <col min="30" max="30" width="20.125" style="2" customWidth="1"/>
+    <col min="31" max="31" width="13.375" style="1" customWidth="1"/>
+    <col min="32" max="32" width="17.75" style="2" customWidth="1"/>
+    <col min="33" max="33" width="12.125" style="2" customWidth="1"/>
+    <col min="34" max="34" width="12.75" style="2" customWidth="1"/>
+    <col min="35" max="35" width="24.375" style="2" customWidth="1"/>
     <col min="36" max="36" width="21" style="2" customWidth="1"/>
-    <col min="37" max="37" width="18.5" style="2" customWidth="1"/>
-    <col min="38" max="38" width="18.25" style="2" customWidth="1"/>
-    <col min="39" max="39" width="18.125" style="2" customWidth="1"/>
-    <col min="40" max="40" width="19.25" style="2" customWidth="1"/>
+    <col min="37" max="37" width="17.375" style="2" customWidth="1"/>
+    <col min="38" max="38" width="17.625" style="2" customWidth="1"/>
+    <col min="39" max="39" width="15.25" style="2" customWidth="1"/>
+    <col min="40" max="40" width="16.875" style="2" customWidth="1"/>
     <col min="41" max="41" width="17.125" style="2" customWidth="1"/>
     <col min="42" max="42" width="19.375" style="2" customWidth="1"/>
     <col min="43" max="43" width="18.375" style="2" customWidth="1"/>
-    <col min="44" max="44" width="16" style="2" customWidth="1"/>
-    <col min="45" max="45" width="19.875" style="2" customWidth="1"/>
-    <col min="46" max="46" width="15.125" style="2" customWidth="1"/>
-    <col min="47" max="47" width="11" style="2" customWidth="1"/>
-    <col min="48" max="48" width="22.125" style="2" customWidth="1"/>
+    <col min="44" max="44" width="15.5" style="2" customWidth="1"/>
+    <col min="45" max="45" width="24.75" style="2" customWidth="1"/>
+    <col min="46" max="46" width="15.25" style="2" customWidth="1"/>
+    <col min="47" max="47" width="17.5" style="2" customWidth="1"/>
+    <col min="48" max="48" width="19.125" style="2" customWidth="1"/>
     <col min="49" max="49" width="18.75" style="2" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="11.375" style="2" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="22.625" style="2" bestFit="1" customWidth="1"/>
@@ -930,54 +931,54 @@
       </c>
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="8"/>
-      <c r="AA15" s="8"/>
-      <c r="AB15" s="8"/>
-      <c r="AC15" s="8"/>
-      <c r="AD15" s="8"/>
-      <c r="AE15" s="8"/>
-      <c r="AF15" s="8"/>
-      <c r="AG15" s="8"/>
-      <c r="AH15" s="8"/>
-      <c r="AI15" s="8"/>
-      <c r="AJ15" s="8"/>
-      <c r="AK15" s="8"/>
-      <c r="AL15" s="8"/>
-      <c r="AM15" s="8"/>
-      <c r="AN15" s="8"/>
-      <c r="AO15" s="8"/>
-      <c r="AP15" s="8"/>
-      <c r="AQ15" s="8"/>
-      <c r="AR15" s="8"/>
-      <c r="AS15" s="8"/>
-      <c r="AT15" s="8"/>
-      <c r="AU15" s="8"/>
-      <c r="AV15" s="8"/>
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15" s="14"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15" s="14"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="Z15"/>
+      <c r="AA15"/>
+      <c r="AB15"/>
+      <c r="AC15"/>
+      <c r="AD15"/>
+      <c r="AE15"/>
+      <c r="AF15"/>
+      <c r="AG15"/>
+      <c r="AH15"/>
+      <c r="AI15"/>
+      <c r="AJ15"/>
+      <c r="AK15"/>
+      <c r="AL15"/>
+      <c r="AM15"/>
+      <c r="AN15"/>
+      <c r="AO15"/>
+      <c r="AP15"/>
+      <c r="AQ15"/>
+      <c r="AR15"/>
+      <c r="AS15"/>
+      <c r="AT15"/>
+      <c r="AU15"/>
+      <c r="AV15"/>
       <c r="AW15" s="8"/>
     </row>
     <row r="16" spans="1:49" x14ac:dyDescent="0.2">
@@ -987,70 +988,70 @@
       <c r="AE16" s="2"/>
     </row>
     <row r="17" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="E17" s="12"/>
+      <c r="E17" s="11"/>
       <c r="T17" s="1"/>
       <c r="U17" s="2"/>
       <c r="AD17" s="1"/>
       <c r="AE17" s="2"/>
     </row>
     <row r="18" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="E18" s="12"/>
+      <c r="E18" s="11"/>
       <c r="T18" s="1"/>
       <c r="U18" s="2"/>
       <c r="AD18" s="1"/>
       <c r="AE18" s="2"/>
     </row>
     <row r="19" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="E19" s="13"/>
+      <c r="E19" s="12"/>
       <c r="T19" s="1"/>
       <c r="U19" s="2"/>
       <c r="AD19" s="1"/>
       <c r="AE19" s="2"/>
     </row>
     <row r="20" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="E20" s="13"/>
+      <c r="E20" s="12"/>
       <c r="T20" s="1"/>
       <c r="U20" s="2"/>
       <c r="AD20" s="1"/>
       <c r="AE20" s="2"/>
     </row>
     <row r="21" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="E21" s="13"/>
+      <c r="E21" s="12"/>
       <c r="T21" s="1"/>
       <c r="U21" s="2"/>
       <c r="AD21" s="1"/>
       <c r="AE21" s="2"/>
     </row>
     <row r="22" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="E22" s="13"/>
+      <c r="E22" s="12"/>
       <c r="T22" s="1"/>
       <c r="U22" s="2"/>
       <c r="AD22" s="1"/>
       <c r="AE22" s="2"/>
     </row>
     <row r="23" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="E23" s="13"/>
+      <c r="E23" s="12"/>
       <c r="T23" s="1"/>
       <c r="U23" s="2"/>
       <c r="AD23" s="1"/>
       <c r="AE23" s="2"/>
     </row>
     <row r="24" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="E24" s="13"/>
+      <c r="E24" s="12"/>
       <c r="T24" s="1"/>
       <c r="U24" s="2"/>
       <c r="AD24" s="1"/>
       <c r="AE24" s="2"/>
     </row>
     <row r="25" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="E25" s="13"/>
+      <c r="E25" s="12"/>
       <c r="T25" s="1"/>
       <c r="U25" s="2"/>
       <c r="AD25" s="1"/>
       <c r="AE25" s="2"/>
     </row>
     <row r="26" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="E26" s="13"/>
+      <c r="E26" s="12"/>
       <c r="T26" s="1"/>
       <c r="U26" s="2"/>
       <c r="AD26" s="1"/>
@@ -1062,7 +1063,7 @@
       <c r="BB26" s="6"/>
     </row>
     <row r="27" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="E27" s="13"/>
+      <c r="E27" s="12"/>
       <c r="T27" s="1"/>
       <c r="U27" s="2"/>
       <c r="AD27" s="1"/>
@@ -1074,7 +1075,7 @@
       <c r="BB27" s="6"/>
     </row>
     <row r="28" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="E28" s="13"/>
+      <c r="E28" s="12"/>
       <c r="T28" s="1"/>
       <c r="U28" s="2"/>
       <c r="AD28" s="1"/>
@@ -1086,7 +1087,7 @@
       <c r="BB28" s="6"/>
     </row>
     <row r="29" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="F29" s="14"/>
+      <c r="F29" s="13"/>
       <c r="AX29" s="5"/>
       <c r="AY29" s="5"/>
       <c r="AZ29" s="5"/>
@@ -1094,7 +1095,7 @@
       <c r="BB29" s="4"/>
     </row>
     <row r="30" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="F30" s="14"/>
+      <c r="F30" s="13"/>
       <c r="AX30" s="5"/>
       <c r="AY30" s="5"/>
       <c r="AZ30" s="5"/>
@@ -1102,7 +1103,7 @@
       <c r="BB30" s="4"/>
     </row>
     <row r="31" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="F31" s="14"/>
+      <c r="F31" s="13"/>
       <c r="AX31" s="5"/>
       <c r="AY31" s="5"/>
       <c r="AZ31" s="5"/>
@@ -1110,7 +1111,7 @@
       <c r="BB31" s="4"/>
     </row>
     <row r="32" spans="5:54" x14ac:dyDescent="0.2">
-      <c r="F32" s="14"/>
+      <c r="F32" s="13"/>
       <c r="AX32" s="5"/>
       <c r="AY32" s="5"/>
       <c r="AZ32" s="5"/>
@@ -1118,7 +1119,7 @@
       <c r="BB32" s="4"/>
     </row>
     <row r="33" spans="6:54" x14ac:dyDescent="0.2">
-      <c r="F33" s="14"/>
+      <c r="F33" s="13"/>
       <c r="AX33" s="5"/>
       <c r="AY33" s="5"/>
       <c r="AZ33" s="5"/>

</xml_diff>

<commit_message>
#3659-PurchaseTrackingReport Module: pabi_procurement_report https://mobileapp.nstda.or.th/redmine/issues/3659 แก้ไข query และเพิ่ม column ใน Excel
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_tracking.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_tracking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aommy\pabi_file\000\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="124">
   <si>
     <t>รายละเอียด</t>
   </si>
@@ -385,6 +385,15 @@
   </si>
   <si>
     <t>Supplier Code</t>
+  </si>
+  <si>
+    <t>PO status</t>
+  </si>
+  <si>
+    <t>สถานะ PO</t>
+  </si>
+  <si>
+    <t>PO close</t>
   </si>
 </sst>
 </file>
@@ -447,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -465,6 +474,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -798,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL34"/>
+  <dimension ref="A1:BN34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="BA4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BI19" sqref="BI19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -864,7 +876,7 @@
     <col min="57" max="57" width="18.25" style="5" customWidth="1"/>
     <col min="58" max="58" width="24.625" style="5" customWidth="1"/>
     <col min="59" max="59" width="18.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="11.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="11.375" style="5" customWidth="1"/>
     <col min="61" max="61" width="22.625" style="5" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="22.375" style="5" bestFit="1" customWidth="1"/>
     <col min="63" max="64" width="22.375" style="5" customWidth="1"/>
@@ -880,62 +892,62 @@
     <col min="74" max="16384" width="9.125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:66" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -943,13 +955,13 @@
       <c r="Y12" s="5"/>
       <c r="AJ12" s="5"/>
     </row>
-    <row r="13" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
       <c r="AJ13" s="5"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:66" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -1124,8 +1136,20 @@
       <c r="BF14" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:59" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="BH14" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="BI14" s="1"/>
+      <c r="BJ14" s="1"/>
+      <c r="BK14" s="1"/>
+      <c r="BL14" s="1"/>
+      <c r="BM14" s="1"/>
+      <c r="BN14" s="1"/>
+    </row>
+    <row r="15" spans="1:66" s="10" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -1300,8 +1324,20 @@
       <c r="BF15" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.2">
+      <c r="BG15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="BH15" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="BI15" s="1"/>
+      <c r="BJ15" s="1"/>
+      <c r="BK15" s="1"/>
+      <c r="BL15" s="1"/>
+      <c r="BM15" s="1"/>
+      <c r="BN15" s="1"/>
+    </row>
+    <row r="16" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>

</xml_diff>

<commit_message>
#3659-Purchase_Tracking_Report Module: pabi_procurement_report https://mobileapp.nstda.or.th/redmine/issues/3659 แก้ไข query และเพิ่ม column ใน Excel
</commit_message>
<xml_diff>
--- a/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_tracking.xlsx
+++ b/pabi_procurement_report/xlsx_template/xlsx_report_pabi_purchase_tracking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aommy\pabi_file\000\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="124">
   <si>
     <t>รายละเอียด</t>
   </si>
@@ -385,13 +385,22 @@
   </si>
   <si>
     <t>Supplier Code</t>
+  </si>
+  <si>
+    <t>PO status</t>
+  </si>
+  <si>
+    <t>สถานะ PO</t>
+  </si>
+  <si>
+    <t>PO close</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,6 +435,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -447,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -466,6 +482,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,11 +818,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BL34"/>
+  <dimension ref="A1:BN34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -864,7 +882,7 @@
     <col min="57" max="57" width="18.25" style="5" customWidth="1"/>
     <col min="58" max="58" width="24.625" style="5" customWidth="1"/>
     <col min="59" max="59" width="18.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="11.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="11.375" style="5" customWidth="1"/>
     <col min="61" max="61" width="22.625" style="5" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="22.375" style="5" bestFit="1" customWidth="1"/>
     <col min="63" max="64" width="22.375" style="5" customWidth="1"/>
@@ -880,62 +898,62 @@
     <col min="74" max="16384" width="9.125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:66" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -943,13 +961,13 @@
       <c r="Y12" s="5"/>
       <c r="AJ12" s="5"/>
     </row>
-    <row r="13" spans="1:59" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:66" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
       <c r="AJ13" s="5"/>
     </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:66" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -1124,8 +1142,20 @@
       <c r="BF14" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:59" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="BG14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="BH14" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="BI14" s="1"/>
+      <c r="BJ14" s="1"/>
+      <c r="BK14" s="1"/>
+      <c r="BL14" s="1"/>
+      <c r="BM14" s="1"/>
+      <c r="BN14" s="1"/>
+    </row>
+    <row r="15" spans="1:66" s="10" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -1300,8 +1330,20 @@
       <c r="BF15" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.2">
+      <c r="BG15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="BH15" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="BI15" s="1"/>
+      <c r="BJ15" s="1"/>
+      <c r="BK15" s="1"/>
+      <c r="BL15" s="1"/>
+      <c r="BM15" s="1"/>
+      <c r="BN15" s="1"/>
+    </row>
+    <row r="16" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1356,6 +1398,7 @@
       <c r="BE16" s="6"/>
       <c r="BF16" s="6"/>
       <c r="BG16" s="7"/>
+      <c r="BH16" s="9"/>
     </row>
     <row r="17" spans="22:64" x14ac:dyDescent="0.2">
       <c r="V17" s="6"/>

</xml_diff>